<commit_message>
function delet transações criada
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\repositorios_github\finance_pessoal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BF1CC9-5918-4C3C-9804-91AE7653B87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8660D23-F610-4CA5-AE81-A8D28F0BAFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4050" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{D3363923-8F54-40BA-B4C8-8736CF3DCF2D}"/>
   </bookViews>
@@ -448,7 +448,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>